<commit_message>
fixed html for clipboard
</commit_message>
<xml_diff>
--- a/output1.xlsx
+++ b/output1.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,11 +15,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00$"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -36,12 +45,12 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <b val="1"/>
       <color rgb="00000000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <b val="1"/>
       <color rgb="00000000"/>
       <sz val="10"/>
     </font>
@@ -66,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -75,11 +84,118 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="00000000"/>
@@ -98,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -106,24 +222,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -486,190 +637,365 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
-    <col width="49" customWidth="1" min="2" max="2"/>
-    <col width="49" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>('Particulars', 'Particulars')</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>('For the three months ended June 30,', '2024')</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>('For the three months ended June 30,', '2023')</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>('Fiscals', '2024')</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>('Fiscals', '2023')</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>('Fiscals', '2022')</t>
+      <c r="A1" s="15" t="n"/>
+      <c r="B1" s="16" t="inlineStr">
+        <is>
+          <t>(in billions of U.S. dollars)</t>
+        </is>
+      </c>
+      <c r="C1" s="16" t="n"/>
+      <c r="D1" s="16" t="inlineStr">
+        <is>
+          <t>Fiscal</t>
+        </is>
+      </c>
+      <c r="E1" s="16" t="n"/>
+      <c r="F1" s="16" t="inlineStr">
+        <is>
+          <t>Percent Increase (Decrease) U.S. Dollars</t>
+        </is>
+      </c>
+      <c r="G1" s="16" t="inlineStr">
+        <is>
+          <t>Percent Increase (Decrease) Local Currency</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>Food Delivery</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>15153.4</v>
-      </c>
-      <c r="C2" s="6" t="n">
-        <v>11926.12</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>51601.25</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>41299.9</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>33913.14</v>
-      </c>
+      <c r="A2" s="15" t="n"/>
+      <c r="B2" s="16" t="n"/>
+      <c r="C2" s="16" t="n"/>
+      <c r="D2" s="16" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E2" s="16" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F2" s="16" t="n"/>
+      <c r="G2" s="16" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Out-of-home Consumption</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>458.52</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>311.25</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>1571.86</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>776.86</v>
-      </c>
-      <c r="F3" s="6" t="n"/>
+      <c r="A3" s="15" t="n"/>
+      <c r="B3" s="17" t="inlineStr">
+        <is>
+          <t>Geographic Markets (1)</t>
+        </is>
+      </c>
+      <c r="C3" s="18" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D3" s="19" t="n">
+        <v>30.3</v>
+      </c>
+      <c r="E3" s="19" t="n">
+        <v>29.1</v>
+      </c>
+      <c r="F3" s="20" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G3" s="20" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
-        <is>
-          <t>Quick Commerce</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>3740.29</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>1797.65</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>9785.5</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>4513.63</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>828.4299999999999</v>
+      <c r="A4" s="15" t="n"/>
+      <c r="B4" s="17" t="n"/>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="D4" s="18" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="F4" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="18" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>Supply Chain and Distribution</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>12682.57</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>9475.809999999999</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>47796.05</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>32863.47</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>14653</v>
+      <c r="A5" s="15" t="n"/>
+      <c r="B5" s="17" t="n"/>
+      <c r="C5" s="18" t="inlineStr">
+        <is>
+          <t>Growth Markets</t>
+        </is>
+      </c>
+      <c r="D5" s="18" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E5" s="18" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="F5" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="18" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>Platform Innovations</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>187.39</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>387.35</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>1719.24</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>3192.1</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>7654.4</v>
+      <c r="A6" s="15" t="n"/>
+      <c r="B6" s="17" t="n"/>
+      <c r="C6" s="17" t="inlineStr">
+        <is>
+          <t>Total Revenues</t>
+        </is>
+      </c>
+      <c r="D6" s="21">
+        <f>D3 + D4 + D5</f>
+        <v/>
+      </c>
+      <c r="E6" s="21">
+        <f>E3 + E4 + E5</f>
+        <v/>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="22" t="n">
+        <v>0.08</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B7" s="7">
-        <f>B2 + B3 + B4 + B5 + B6</f>
+      <c r="A7" s="15" t="n"/>
+      <c r="B7" s="17" t="inlineStr">
+        <is>
+          <t>Industry Groups</t>
+        </is>
+      </c>
+      <c r="C7" s="18" t="inlineStr">
+        <is>
+          <t>Communications, Media &amp; Technology</t>
+        </is>
+      </c>
+      <c r="D7" s="19" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="F7" s="20" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="G7" s="20" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="n"/>
+      <c r="B8" s="17" t="n"/>
+      <c r="C8" s="18" t="inlineStr">
+        <is>
+          <t>Financial Services</t>
+        </is>
+      </c>
+      <c r="D8" s="18" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="E8" s="18" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="F8" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="n"/>
+      <c r="B9" s="17" t="n"/>
+      <c r="C9" s="18" t="inlineStr">
+        <is>
+          <t>Health &amp; Public Service</t>
+        </is>
+      </c>
+      <c r="D9" s="18" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="E9" s="18" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="F9" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" s="18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="n"/>
+      <c r="B10" s="17" t="n"/>
+      <c r="C10" s="18" t="inlineStr">
+        <is>
+          <t>Products</t>
+        </is>
+      </c>
+      <c r="D10" s="18" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="E10" s="18" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="F10" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="15" t="n"/>
+      <c r="B11" s="17" t="n"/>
+      <c r="C11" s="18" t="inlineStr">
+        <is>
+          <t>Resources</t>
+        </is>
+      </c>
+      <c r="D11" s="18" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E11" s="18" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="F11" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="18" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="n"/>
+      <c r="B12" s="17" t="n"/>
+      <c r="C12" s="17" t="inlineStr">
+        <is>
+          <t>Total Revenues</t>
+        </is>
+      </c>
+      <c r="D12" s="21">
+        <f>D6</f>
         <v/>
       </c>
-      <c r="C7" s="7">
-        <f>C2 + C3 + C4 + C5 + C6</f>
+      <c r="E12" s="21">
+        <f>E6</f>
         <v/>
       </c>
-      <c r="D7" s="7">
-        <f>D2 + D3 + D4 + D5 + D6</f>
+      <c r="F12" s="22" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G12" s="22" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="n"/>
+      <c r="B13" s="17" t="inlineStr">
+        <is>
+          <t>Type of Work</t>
+        </is>
+      </c>
+      <c r="C13" s="18" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="D13" s="19" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="E13" s="19" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="F13" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="20" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="n"/>
+      <c r="B14" s="17" t="n"/>
+      <c r="C14" s="17" t="inlineStr">
+        <is>
+          <t>Managed Services (2)</t>
+        </is>
+      </c>
+      <c r="D14" s="17">
+        <f>D12 - D13</f>
         <v/>
       </c>
-      <c r="E7" s="7">
-        <f>E2 + E3 + E4 + E5 + E6</f>
+      <c r="E14" s="17">
+        <f>E12 - E13</f>
         <v/>
       </c>
-      <c r="F7" s="7">
-        <f>F2 + F3 + F4 + F5 + F6</f>
-        <v/>
+      <c r="F14" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="15" t="n"/>
+      <c r="B15" s="17" t="n"/>
+      <c r="C15" s="18" t="inlineStr">
+        <is>
+          <t>Total Revenues</t>
+        </is>
+      </c>
+      <c r="D15" s="19" t="n">
+        <v>64.09999999999999</v>
+      </c>
+      <c r="E15" s="19" t="n">
+        <v>61.6</v>
+      </c>
+      <c r="F15" s="20" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G15" s="20" t="n">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="7">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>